<commit_message>
Adding signal and battery tests for appium
</commit_message>
<xml_diff>
--- a/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/EBManual_Notification_JS.xlsx
+++ b/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/EBManual_Notification_JS.xlsx
@@ -1087,23 +1087,6 @@
 };</t>
   </si>
   <si>
-    <t>wait(5);
-validate1;
-link_Click(notification_test_link);
-validate2;
-SelectTestToRun(VT307_0043_string);
-ClickRunTest(runtest_top_xpath);
-wait(2);
-validate3;
-ClickRunTest(runtest_bottom_xpath);
-wait(2);
-SwipeNotification(EnterpriseBrowser);
-TapNotification(EnterpriseBrowser);
-CheckUITextContains(Test_Message);
-ClickUIButtonText(ok);
-validate5;</t>
-  </si>
-  <si>
     <t>validate1
 {
 validate_PageTitle=Manual specs
@@ -1124,23 +1107,6 @@
 };</t>
   </si>
   <si>
-    <t>wait(5);
-validate1;
-link_Click(notification_test_link);
-validate2;
-SelectTestToRun(VT307_0044_string);
-ClickRunTest(runtest_top_xpath);
-wait(2);
-validate3;
-ClickRunTest(runtest_bottom_xpath);
-wait(2);
-SwipeNotification(EnterpriseBrowser);
-TapNotification(EnterpriseBrowser);
-CheckUITextContains(Test_Message);
-ClickUIButtonText(ok);
-validate5;</t>
-  </si>
-  <si>
     <t xml:space="preserve">validate1
 {
 validate_PageTitle=Manual specs
@@ -1162,23 +1128,6 @@
 </t>
   </si>
   <si>
-    <t>wait(5);
-validate1;
-link_Click(notification_test_link);
-validate2;
-SelectTestToRun(VT307_0045_string);
-ClickRunTest(runtest_top_xpath);
-wait(2);
-validate3;
-ClickRunTest(runtest_bottom_xpath);
-wait(2);
-SwipeNotification(EnterpriseBrowser);
-TapNotification(EnterpriseBrowser);
-CheckUITextContains(Test_Message);
-ClickUIButtonText(ok);
-validate5;</t>
-  </si>
-  <si>
     <t xml:space="preserve">validate1
 {
 validate_PageTitle=Manual specs
@@ -1198,23 +1147,6 @@
 validate_Result="button_index":"0"
 };
 </t>
-  </si>
-  <si>
-    <t>wait(5);
-validate1;
-link_Click(notification_test_link);
-validate2;
-SelectTestToRun(VT307_0046_string);
-ClickRunTest(runtest_top_xpath);
-wait(2);
-validate3;
-ClickRunTest(runtest_bottom_xpath);
-wait(2);
-SwipeNotification(EnterpriseBrowser);
-TapNotification(EnterpriseBrowser);
-CheckUITextContains(Test_Message);
-ClickUIButtonText(ok);
-validate5;</t>
   </si>
   <si>
     <t xml:space="preserve">validate1
@@ -1251,6 +1183,74 @@
 UIAutomatorScreenshot(VT307_0056);
 validate4;
 ClickUIButtonText(yes);</t>
+  </si>
+  <si>
+    <t>wait(5);
+validate1;
+link_Click(notification_test_link);
+validate2;
+SelectTestToRun(VT307_0043_string);
+ClickRunTest(runtest_top_xpath);
+wait(2);
+validate3;
+ClickRunTest(runtest_bottom_xpath);
+wait(2);
+SwipeNotification(Displaying_a_pop_up);
+TapNotification(Displaying_a_pop_up);
+CheckUITextContains(Test_Message);
+ClickUIButtonText(ok);
+validate5;</t>
+  </si>
+  <si>
+    <t>wait(5);
+validate1;
+link_Click(notification_test_link);
+validate2;
+SelectTestToRun(VT307_0044_string);
+ClickRunTest(runtest_top_xpath);
+wait(2);
+validate3;
+ClickRunTest(runtest_bottom_xpath);
+wait(2);
+SwipeNotification(Displaying_a_pop_up);
+TapNotification(Displaying_a_pop_up);
+CheckUITextContains(Test_Message);
+ClickUIButtonText(ok);
+validate5;</t>
+  </si>
+  <si>
+    <t>wait(5);
+validate1;
+link_Click(notification_test_link);
+validate2;
+SelectTestToRun(VT307_0045_string);
+ClickRunTest(runtest_top_xpath);
+wait(2);
+validate3;
+ClickRunTest(runtest_bottom_xpath);
+wait(2);
+SwipeNotification(Displaying_a_pop_up);
+TapNotification(Displaying_a_pop_up);
+CheckUITextContains(Test_Message);
+ClickUIButtonText(ok);
+validate5;</t>
+  </si>
+  <si>
+    <t>wait(5);
+validate1;
+link_Click(notification_test_link);
+validate2;
+SelectTestToRun(VT307_0046_string);
+ClickRunTest(runtest_top_xpath);
+wait(2);
+validate3;
+ClickRunTest(runtest_bottom_xpath);
+wait(2);
+SwipeNotification(Displaying_a_pop_up);
+TapNotification(Displaying_a_pop_up);
+CheckUITextContains(Test_Message);
+ClickUIButtonText(ok);
+validate5;</t>
   </si>
 </sst>
 </file>
@@ -1762,7 +1762,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -2448,10 +2450,10 @@
       </c>
       <c r="F26" s="13"/>
       <c r="G26" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="H26" s="13" t="s">
         <v>109</v>
-      </c>
-      <c r="H26" s="13" t="s">
-        <v>110</v>
       </c>
       <c r="I26" s="11"/>
       <c r="J26" s="11"/>
@@ -2472,10 +2474,10 @@
       </c>
       <c r="F27" s="13"/>
       <c r="G27" s="13" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="H27" s="13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I27" s="11"/>
       <c r="J27" s="11"/>
@@ -2496,10 +2498,10 @@
       </c>
       <c r="F28" s="13"/>
       <c r="G28" s="13" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="H28" s="13" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="I28" s="11"/>
       <c r="J28" s="11"/>
@@ -2520,10 +2522,10 @@
       </c>
       <c r="F29" s="11"/>
       <c r="G29" s="13" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="H29" s="13" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="I29" s="11"/>
       <c r="J29" s="11"/>
@@ -2594,7 +2596,7 @@
       </c>
       <c r="F32" s="11"/>
       <c r="G32" s="13" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="H32" s="13" t="s">
         <v>99</v>

</xml_diff>